<commit_message>
mitch final version including preliminary pca + mlr
</commit_message>
<xml_diff>
--- a/median_plane/points_for_median_plane.xlsx
+++ b/median_plane/points_for_median_plane.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIPAG_~1\AppData\Local\Temp\Mxt214\RemoteFiles\395372_3_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIPAG_~1\AppData\Local\Temp\Mxt214\RemoteFiles\263658_3_49\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="129">
   <si>
     <t>Cohort</t>
   </si>
@@ -445,6 +445,12 @@
     <t>4A
 z</t>
   </si>
+  <si>
+    <t>Scaled all by ---&gt;</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
 </sst>
 </file>
 
@@ -587,7 +593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -766,92 +772,15 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1212,13 +1141,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO170"/>
+  <dimension ref="A1:AP170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1:AJ1"/>
+      <selection pane="bottomRight" activeCell="AJ65" sqref="AJ65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,32 +1161,35 @@
     <col min="8" max="8" width="5.5703125" style="23" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="5" style="27" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="4.42578125" style="43" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.5703125" style="43" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="4.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5" style="41" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5" style="41" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5" style="41" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="3" customWidth="1"/>
-    <col min="38" max="38" width="13.28515625" customWidth="1"/>
-    <col min="39" max="40" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.42578125" customWidth="1"/>
+    <col min="39" max="39" width="9.140625" customWidth="1"/>
+    <col min="40" max="40" width="8.5703125" customWidth="1"/>
+    <col min="41" max="41" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="3.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>82</v>
       </c>
@@ -1366,11 +1298,11 @@
       <c r="AJ1" s="48" t="s">
         <v>126</v>
       </c>
+      <c r="AM1" s="10" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -1464,17 +1396,17 @@
       <c r="AJ2" s="28">
         <v>534</v>
       </c>
-      <c r="AM2" s="42">
+      <c r="AN2" s="42">
         <v>637</v>
       </c>
-      <c r="AN2" s="42">
+      <c r="AO2" s="42">
         <v>362</v>
       </c>
-      <c r="AO2" s="42">
+      <c r="AP2" s="42">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -1568,17 +1500,17 @@
       <c r="AJ3" s="28">
         <v>430</v>
       </c>
-      <c r="AM3" s="43">
+      <c r="AN3" s="43">
         <v>555</v>
       </c>
-      <c r="AN3" s="43">
+      <c r="AO3" s="43">
         <v>406</v>
       </c>
-      <c r="AO3" s="43">
+      <c r="AP3" s="43">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1672,17 +1604,17 @@
       <c r="AJ4" s="28">
         <v>570</v>
       </c>
-      <c r="AM4" s="42">
+      <c r="AN4" s="42">
         <v>603</v>
       </c>
-      <c r="AN4" s="42">
+      <c r="AO4" s="42">
         <v>387</v>
       </c>
-      <c r="AO4" s="42">
+      <c r="AP4" s="42">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1776,17 +1708,17 @@
       <c r="AJ5" s="28">
         <v>482</v>
       </c>
-      <c r="AM5" s="42">
+      <c r="AN5" s="42">
         <v>602</v>
       </c>
-      <c r="AN5" s="42">
+      <c r="AO5" s="42">
         <v>402</v>
       </c>
-      <c r="AO5" s="42">
+      <c r="AP5" s="42">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1880,17 +1812,17 @@
       <c r="AJ6" s="28">
         <v>603</v>
       </c>
-      <c r="AM6" s="42">
+      <c r="AN6" s="42">
         <v>637</v>
       </c>
-      <c r="AN6" s="42">
+      <c r="AO6" s="42">
         <v>399</v>
       </c>
-      <c r="AO6" s="42">
+      <c r="AP6" s="42">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -1987,11 +1919,11 @@
       <c r="AL7" t="s">
         <v>100</v>
       </c>
-      <c r="AM7" s="42"/>
       <c r="AN7" s="42"/>
       <c r="AO7" s="42"/>
+      <c r="AP7" s="42"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -2085,17 +2017,17 @@
       <c r="AJ8" s="28">
         <v>526</v>
       </c>
-      <c r="AM8" s="42">
+      <c r="AN8" s="42">
         <v>600</v>
       </c>
-      <c r="AN8" s="42">
+      <c r="AO8" s="42">
         <v>389</v>
       </c>
-      <c r="AO8" s="42">
+      <c r="AP8" s="42">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -2189,17 +2121,17 @@
       <c r="AJ9" s="28">
         <v>534</v>
       </c>
-      <c r="AM9" s="42">
+      <c r="AN9" s="42">
         <v>585</v>
       </c>
-      <c r="AN9" s="42">
+      <c r="AO9" s="42">
         <v>419</v>
       </c>
-      <c r="AO9" s="42">
+      <c r="AP9" s="42">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -2293,17 +2225,17 @@
       <c r="AJ10" s="28">
         <v>547</v>
       </c>
-      <c r="AM10" s="42">
+      <c r="AN10" s="42">
         <v>613</v>
       </c>
-      <c r="AN10" s="42">
+      <c r="AO10" s="42">
         <v>395</v>
       </c>
-      <c r="AO10" s="42">
+      <c r="AP10" s="42">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>3</v>
       </c>
@@ -2397,17 +2329,17 @@
       <c r="AJ11" s="28">
         <v>539</v>
       </c>
-      <c r="AM11" s="42">
+      <c r="AN11" s="42">
         <v>654</v>
       </c>
-      <c r="AN11" s="42">
+      <c r="AO11" s="42">
         <v>376</v>
       </c>
-      <c r="AO11" s="42">
+      <c r="AP11" s="42">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -2501,17 +2433,17 @@
       <c r="AJ12" s="28">
         <v>534</v>
       </c>
-      <c r="AM12" s="42">
+      <c r="AN12" s="42">
         <v>620</v>
       </c>
-      <c r="AN12" s="42">
+      <c r="AO12" s="42">
         <v>377</v>
       </c>
-      <c r="AO12" s="42">
+      <c r="AP12" s="42">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -2605,17 +2537,17 @@
       <c r="AJ13" s="28">
         <v>499</v>
       </c>
-      <c r="AM13" s="42">
+      <c r="AN13" s="42">
         <v>629</v>
       </c>
-      <c r="AN13" s="42">
+      <c r="AO13" s="42">
         <v>370</v>
       </c>
-      <c r="AO13" s="42">
+      <c r="AP13" s="42">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>3</v>
       </c>
@@ -2709,11 +2641,11 @@
       <c r="AJ14" s="28">
         <v>522</v>
       </c>
-      <c r="AM14" s="42"/>
       <c r="AN14" s="42"/>
       <c r="AO14" s="42"/>
+      <c r="AP14" s="42"/>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -2807,17 +2739,17 @@
       <c r="AJ15" s="28">
         <v>466</v>
       </c>
-      <c r="AM15" s="42">
+      <c r="AN15" s="42">
         <v>604</v>
       </c>
-      <c r="AN15" s="42">
+      <c r="AO15" s="42">
         <v>395</v>
       </c>
-      <c r="AO15" s="42">
+      <c r="AP15" s="42">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -2911,17 +2843,17 @@
       <c r="AJ16" s="28">
         <v>547</v>
       </c>
-      <c r="AM16" s="42">
+      <c r="AN16" s="42">
         <v>605</v>
       </c>
-      <c r="AN16" s="42">
+      <c r="AO16" s="42">
         <v>419</v>
       </c>
-      <c r="AO16" s="42">
+      <c r="AP16" s="42">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -3015,17 +2947,17 @@
       <c r="AJ17" s="28">
         <v>474</v>
       </c>
-      <c r="AM17" s="42">
+      <c r="AN17" s="42">
         <v>358</v>
       </c>
-      <c r="AN17" s="42">
+      <c r="AO17" s="42">
         <v>389</v>
       </c>
-      <c r="AO17" s="42">
+      <c r="AP17" s="42">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -3119,17 +3051,17 @@
       <c r="AJ18" s="28">
         <v>541</v>
       </c>
-      <c r="AM18" s="42">
+      <c r="AN18" s="42">
         <v>609</v>
       </c>
-      <c r="AN18" s="42">
+      <c r="AO18" s="42">
         <v>392</v>
       </c>
-      <c r="AO18" s="42">
+      <c r="AP18" s="42">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -3227,7 +3159,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="20" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>3</v>
       </c>
@@ -3325,7 +3257,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="21" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -3417,7 +3349,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="22" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>3</v>
       </c>
@@ -3515,7 +3447,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="23" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -3613,7 +3545,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="24" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>3</v>
       </c>
@@ -3705,7 +3637,7 @@
       <c r="AI24" s="33"/>
       <c r="AJ24" s="28"/>
     </row>
-    <row r="25" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>3</v>
       </c>
@@ -3803,7 +3735,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="26" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -3901,7 +3833,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="27" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>3</v>
       </c>
@@ -3993,7 +3925,7 @@
       <c r="AI27" s="33"/>
       <c r="AJ27" s="28"/>
     </row>
-    <row r="28" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>3</v>
       </c>
@@ -4091,7 +4023,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="29" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -4189,7 +4121,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="30" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -4283,17 +4215,17 @@
       <c r="AJ30" s="28">
         <v>525</v>
       </c>
-      <c r="AM30" s="42">
+      <c r="AN30" s="42">
         <v>521</v>
       </c>
-      <c r="AN30" s="42">
+      <c r="AO30" s="42">
         <v>397</v>
       </c>
-      <c r="AO30" s="42">
+      <c r="AP30" s="42">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>3</v>
       </c>
@@ -4387,11 +4319,11 @@
       <c r="AJ31" s="28">
         <v>518</v>
       </c>
-      <c r="AM31" s="42"/>
       <c r="AN31" s="42"/>
       <c r="AO31" s="42"/>
+      <c r="AP31" s="42"/>
     </row>
-    <row r="32" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>3</v>
       </c>
@@ -4485,11 +4417,11 @@
       <c r="AJ32" s="28">
         <v>504</v>
       </c>
-      <c r="AM32" s="42"/>
       <c r="AN32" s="42"/>
       <c r="AO32" s="42"/>
+      <c r="AP32" s="42"/>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>3</v>
       </c>
@@ -4583,11 +4515,11 @@
       <c r="AJ33" s="28">
         <v>604</v>
       </c>
-      <c r="AM33" s="42"/>
       <c r="AN33" s="42"/>
       <c r="AO33" s="42"/>
+      <c r="AP33" s="42"/>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>3</v>
       </c>
@@ -4681,11 +4613,11 @@
       <c r="AJ34" s="28">
         <v>516</v>
       </c>
-      <c r="AM34" s="42"/>
       <c r="AN34" s="42"/>
       <c r="AO34" s="42"/>
+      <c r="AP34" s="42"/>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>3</v>
       </c>
@@ -4779,17 +4711,17 @@
       <c r="AJ35" s="28">
         <v>537</v>
       </c>
-      <c r="AM35" s="42">
+      <c r="AN35" s="42">
         <v>632</v>
       </c>
-      <c r="AN35" s="42">
+      <c r="AO35" s="42">
         <v>360</v>
       </c>
-      <c r="AO35" s="42">
+      <c r="AP35" s="42">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>3</v>
       </c>
@@ -4887,7 +4819,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>3</v>
       </c>
@@ -4985,7 +4917,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>3</v>
       </c>
@@ -5083,7 +5015,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -5181,7 +5113,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -5279,7 +5211,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>3</v>
       </c>
@@ -5377,7 +5309,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>3</v>
       </c>
@@ -5475,7 +5407,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>3</v>
       </c>
@@ -5573,7 +5505,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>3</v>
       </c>
@@ -5671,7 +5603,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>3</v>
       </c>
@@ -5769,7 +5701,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>3</v>
       </c>
@@ -5867,7 +5799,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>3</v>
       </c>
@@ -5965,7 +5897,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="48" spans="1:41" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="4" t="s">
         <v>3</v>
@@ -6065,7 +5997,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B49" s="20" t="s">
         <v>4</v>
       </c>
@@ -6163,7 +6095,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>4</v>
       </c>
@@ -6261,7 +6193,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>4</v>
       </c>
@@ -6359,7 +6291,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>4</v>
       </c>
@@ -6457,7 +6389,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>4</v>
       </c>
@@ -6555,7 +6487,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>4</v>
       </c>
@@ -6653,7 +6585,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>4</v>
       </c>
@@ -6751,7 +6683,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>4</v>
       </c>
@@ -6849,7 +6781,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="57" spans="1:36" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:40" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="49" t="s">
         <v>4</v>
@@ -6949,7 +6881,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>4</v>
       </c>
@@ -7047,7 +6979,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B59" s="49" t="s">
         <v>4</v>
       </c>
@@ -7145,7 +7077,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B60" s="49" t="s">
         <v>4</v>
       </c>
@@ -7243,7 +7175,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B61" s="49" t="s">
         <v>4</v>
       </c>
@@ -7341,7 +7273,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B62" s="49" t="s">
         <v>4</v>
       </c>
@@ -7439,7 +7371,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B63" s="49" t="s">
         <v>4</v>
       </c>
@@ -7537,8 +7469,10 @@
         <v>665</v>
       </c>
     </row>
-    <row r="64" spans="1:36" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
+    <row r="64" spans="1:40" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>1</v>
+      </c>
       <c r="B64" s="49" t="s">
         <v>4</v>
       </c>
@@ -7570,80 +7504,112 @@
         <v>0.5</v>
       </c>
       <c r="L64" s="19"/>
-      <c r="M64" s="39">
+      <c r="M64" s="18">
+        <f>118*AM64</f>
         <v>118</v>
       </c>
-      <c r="N64" s="35">
+      <c r="N64" s="18">
+        <f>271*AM64</f>
         <v>271</v>
       </c>
-      <c r="O64" s="35">
+      <c r="O64" s="18">
+        <f>80*AM64</f>
         <v>80</v>
       </c>
-      <c r="P64" s="35">
+      <c r="P64" s="18">
+        <f>404*AM64</f>
         <v>404</v>
       </c>
-      <c r="Q64" s="35">
+      <c r="Q64" s="18">
+        <f>263*AM64</f>
         <v>263</v>
       </c>
-      <c r="R64" s="35">
+      <c r="R64" s="18">
+        <f>80*AM64</f>
         <v>80</v>
       </c>
-      <c r="S64" s="39">
+      <c r="S64" s="18">
+        <f>76*AM64</f>
         <v>76</v>
       </c>
-      <c r="T64" s="35">
+      <c r="T64" s="18">
+        <f>256*AM64</f>
         <v>256</v>
       </c>
-      <c r="U64" s="35">
+      <c r="U64" s="18">
+        <f>241*AM64</f>
         <v>241</v>
       </c>
-      <c r="V64" s="35">
+      <c r="V64" s="18">
+        <f>439*AM64</f>
         <v>439</v>
       </c>
-      <c r="W64" s="35">
+      <c r="W64" s="18">
+        <f>261*AM64</f>
         <v>261</v>
       </c>
-      <c r="X64" s="35">
+      <c r="X64" s="18">
+        <f>241*AM64</f>
         <v>241</v>
       </c>
-      <c r="Y64" s="39">
+      <c r="Y64" s="18">
+        <f>75*AM64</f>
         <v>75</v>
       </c>
-      <c r="Z64" s="35">
+      <c r="Z64" s="18">
+        <f>242*AM64</f>
         <v>242</v>
       </c>
-      <c r="AA64" s="35">
+      <c r="AA64" s="18">
+        <f>402*AM64</f>
         <v>402</v>
       </c>
-      <c r="AB64" s="35">
+      <c r="AB64" s="18">
+        <f>421*AM64</f>
         <v>421</v>
       </c>
-      <c r="AC64" s="35">
+      <c r="AC64" s="18">
+        <f>244*AM64</f>
         <v>244</v>
       </c>
-      <c r="AD64" s="35">
+      <c r="AD64" s="18">
+        <f>402*AM64</f>
         <v>402</v>
       </c>
-      <c r="AE64" s="39">
+      <c r="AE64" s="18">
+        <f>96*AM64</f>
         <v>96</v>
       </c>
-      <c r="AF64" s="35">
+      <c r="AF64" s="18">
+        <f>240*AM64</f>
         <v>240</v>
       </c>
-      <c r="AG64" s="35">
+      <c r="AG64" s="18">
+        <f>563*AM64</f>
         <v>563</v>
       </c>
-      <c r="AH64" s="35">
+      <c r="AH64" s="18">
+        <f>353*AM64</f>
         <v>353</v>
       </c>
-      <c r="AI64" s="35">
+      <c r="AI64" s="18">
+        <f>242*AM64</f>
         <v>242</v>
       </c>
-      <c r="AJ64" s="30">
+      <c r="AJ64" s="18">
+        <f>563*AM64</f>
         <v>563</v>
       </c>
+      <c r="AL64" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM64" s="18">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="AN64" s="66"/>
     </row>
-    <row r="65" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B65" s="49" t="s">
         <v>4</v>
       </c>
@@ -7735,7 +7701,7 @@
       <c r="AI65" s="33"/>
       <c r="AJ65" s="28"/>
     </row>
-    <row r="66" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B66" s="49" t="s">
         <v>4</v>
       </c>
@@ -7829,17 +7795,17 @@
       <c r="AJ66" s="28">
         <v>659</v>
       </c>
-      <c r="AM66" s="42">
+      <c r="AN66" s="42">
         <v>436</v>
       </c>
-      <c r="AN66" s="42">
+      <c r="AO66" s="42">
         <v>259</v>
       </c>
-      <c r="AO66" s="42">
+      <c r="AP66" s="42">
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B67" s="49" t="s">
         <v>4</v>
       </c>
@@ -7937,7 +7903,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="68" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B68" s="49" t="s">
         <v>4</v>
       </c>
@@ -8035,7 +8001,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="69" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B69" s="49" t="s">
         <v>4</v>
       </c>
@@ -8133,7 +8099,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="70" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B70" s="49" t="s">
         <v>4</v>
       </c>
@@ -8231,7 +8197,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="71" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B71" s="49" t="s">
         <v>4</v>
       </c>
@@ -8329,7 +8295,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="72" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B72" s="49" t="s">
         <v>4</v>
       </c>
@@ -8427,7 +8393,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="73" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B73" s="49" t="s">
         <v>4</v>
       </c>
@@ -8525,7 +8491,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="74" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B74" s="49" t="s">
         <v>4</v>
       </c>
@@ -8623,7 +8589,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="75" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B75" s="49" t="s">
         <v>4</v>
       </c>
@@ -8721,7 +8687,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="76" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B76" s="49" t="s">
         <v>4</v>
       </c>
@@ -8819,7 +8785,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="77" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B77" s="49" t="s">
         <v>4</v>
       </c>
@@ -8917,7 +8883,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="78" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B78" s="49" t="s">
         <v>4</v>
       </c>
@@ -9015,7 +8981,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="79" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B79" s="49" t="s">
         <v>4</v>
       </c>
@@ -9113,7 +9079,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="80" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B80" s="49" t="s">
         <v>4</v>
       </c>
@@ -9211,7 +9177,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B81" s="49" t="s">
         <v>4</v>
       </c>
@@ -9309,7 +9275,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B82" s="49" t="s">
         <v>4</v>
       </c>
@@ -9403,17 +9369,17 @@
       <c r="AJ82" s="28">
         <v>490</v>
       </c>
-      <c r="AM82" s="42">
+      <c r="AN82" s="42">
         <v>414</v>
       </c>
-      <c r="AN82" s="42">
+      <c r="AO82" s="42">
         <v>248</v>
       </c>
-      <c r="AO82" s="42">
+      <c r="AP82" s="42">
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="50" t="s">
         <v>4</v>
@@ -9513,7 +9479,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="84" spans="1:41" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="4" t="s">
         <v>4</v>
@@ -9607,7 +9573,7 @@
       <c r="AI84" s="34"/>
       <c r="AJ84" s="29"/>
     </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>3</v>
       </c>
@@ -9711,7 +9677,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>3</v>
       </c>
@@ -9815,7 +9781,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>3</v>
       </c>
@@ -9913,7 +9879,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>3</v>
       </c>
@@ -10011,7 +9977,7 @@
       <c r="AI88" s="33"/>
       <c r="AJ88" s="28"/>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>3</v>
       </c>
@@ -10115,7 +10081,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B90" s="60" t="s">
         <v>3</v>
       </c>
@@ -10158,8 +10124,9 @@
       <c r="AL90" s="57" t="s">
         <v>102</v>
       </c>
+      <c r="AM90" s="57"/>
     </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>3</v>
       </c>
@@ -10263,7 +10230,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>3</v>
       </c>
@@ -10367,7 +10334,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>3</v>
       </c>
@@ -10463,7 +10430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>3</v>
       </c>
@@ -10567,7 +10534,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>3</v>
       </c>
@@ -10665,7 +10632,7 @@
       <c r="AI95" s="33"/>
       <c r="AJ95" s="28"/>
     </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>3</v>
       </c>
@@ -13971,7 +13938,7 @@
       <c r="AI128" s="33"/>
       <c r="AJ128" s="28"/>
     </row>
-    <row r="129" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>3</v>
       </c>
@@ -14063,7 +14030,7 @@
       <c r="AI129" s="33"/>
       <c r="AJ129" s="28"/>
     </row>
-    <row r="130" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>3</v>
       </c>
@@ -14161,7 +14128,7 @@
       <c r="AI130" s="33"/>
       <c r="AJ130" s="28"/>
     </row>
-    <row r="131" spans="1:38" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="4" t="s">
         <v>3</v>
@@ -14267,7 +14234,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="132" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B132" s="20" t="s">
         <v>4</v>
       </c>
@@ -14310,8 +14277,9 @@
       <c r="AL132" s="57" t="s">
         <v>102</v>
       </c>
+      <c r="AM132" s="57"/>
     </row>
-    <row r="133" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>4</v>
       </c>
@@ -14409,7 +14377,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="134" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>4</v>
       </c>
@@ -14501,7 +14469,7 @@
       <c r="AI134" s="33"/>
       <c r="AJ134" s="28"/>
     </row>
-    <row r="135" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>4</v>
       </c>
@@ -14599,7 +14567,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="136" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>4</v>
       </c>
@@ -14697,7 +14665,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="137" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>4</v>
       </c>
@@ -14795,7 +14763,7 @@
       <c r="AI137" s="33"/>
       <c r="AJ137" s="28"/>
     </row>
-    <row r="138" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>4</v>
       </c>
@@ -14893,7 +14861,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="139" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>4</v>
       </c>
@@ -14991,7 +14959,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="140" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>4</v>
       </c>
@@ -15083,7 +15051,7 @@
       <c r="AI140" s="33"/>
       <c r="AJ140" s="28"/>
     </row>
-    <row r="141" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>4</v>
       </c>
@@ -15175,7 +15143,7 @@
       <c r="AI141" s="33"/>
       <c r="AJ141" s="28"/>
     </row>
-    <row r="142" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>4</v>
       </c>
@@ -15267,7 +15235,7 @@
       <c r="AI142" s="33"/>
       <c r="AJ142" s="28"/>
     </row>
-    <row r="143" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>4</v>
       </c>
@@ -15371,7 +15339,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="144" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>4</v>
       </c>
@@ -17756,22 +17724,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W1:X1">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:AD1">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:R1">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI1:AJ1">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>